<commit_message>
added hydrogen emissions to glass input file
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_glass_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_glass_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="8_{88BDB2A0-9F3B-41BA-AFFE-064AABA643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D253FD3-5B9F-469E-9A2B-E8324DD846BD}"/>
+  <xr:revisionPtr revIDLastSave="215" documentId="8_{88BDB2A0-9F3B-41BA-AFFE-064AABA643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{306F301C-870A-4071-B828-5951F4733EBF}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Nom</t>
   </si>
@@ -552,7 +552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A1527-08E9-4208-98F7-539760163740}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -940,10 +940,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDE4F52-1213-4E96-AFE3-14D53043F5A9}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,7 +1047,91 @@
         <v>0</v>
       </c>
       <c r="D7" s="5">
-        <v>0</v>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2050</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2050</v>
+      </c>
+      <c r="C9">
+        <v>44</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>2050</v>
+      </c>
+      <c r="C10">
+        <v>272</v>
+      </c>
+      <c r="D10">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>2050</v>
+      </c>
+      <c r="C11">
+        <v>27</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>2050</v>
+      </c>
+      <c r="C12">
+        <v>346.5</v>
+      </c>
+      <c r="D12">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>2050</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new paper pulp input file
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_glass_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_glass_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="215" documentId="8_{88BDB2A0-9F3B-41BA-AFFE-064AABA643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{306F301C-870A-4071-B828-5951F4733EBF}"/>
+  <xr:revisionPtr revIDLastSave="257" documentId="8_{88BDB2A0-9F3B-41BA-AFFE-064AABA643B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25CE5CE7-3D52-4AC2-8835-DFEC5093E903}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
   <si>
     <t>Nom</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>conso_unitaire_hydrogen</t>
+  </si>
+  <si>
+    <t>seasonal_efficiency</t>
   </si>
 </sst>
 </file>
@@ -220,7 +223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -234,7 +237,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A1527-08E9-4208-98F7-539760163740}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -688,7 +693,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection sqref="A1:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,10 +945,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDE4F52-1213-4E96-AFE3-14D53043F5A9}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,187 +956,226 @@
     <col min="3" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0</v>
+      </c>
+      <c r="D2" s="5">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="E2" s="5">
+        <v>0.55879999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>2020</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="5">
         <v>187</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <f>227-C3</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" s="5">
+        <v>0.4536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>2020</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="5">
         <v>272</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>2020</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="5">
         <v>27</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>2020</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="5">
         <v>346.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="E6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7">
-        <v>2020</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
+      <c r="B7" s="5">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
         <v>289</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="E7" s="5">
+        <v>0.4536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>2050</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="E8" s="5">
+        <v>0.66612401833447832</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>2050</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>44</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="D9" s="5">
+        <v>0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.53659990365832977</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>2050</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>272</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>57</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>2050</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>27</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>2050</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>346.5</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>2050</v>
       </c>
-      <c r="C13" s="5">
-        <v>0</v>
-      </c>
-      <c r="D13" s="5">
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
         <v>15</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.53659990365832977</v>
       </c>
     </row>
   </sheetData>
@@ -1145,7 +1189,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>